<commit_message>
Se agregan tablas para casos de pruebas
</commit_message>
<xml_diff>
--- a/casos de prueba/casos de prueba.xlsx
+++ b/casos de prueba/casos de prueba.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbeja\Desktop\EntregaFinalCoder\Entrega_final_CodeHouse_Python\casos de prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1A5820-6046-46D1-B9B9-A8A63B3ECB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC423438-1019-4083-805A-CB8D3DE609DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{216521C0-8688-43E0-9A96-A5931696C490}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{216521C0-8688-43E0-9A96-A5931696C490}"/>
   </bookViews>
   <sheets>
     <sheet name="Crud blog" sheetId="1" r:id="rId1"/>
+    <sheet name="prueba 2" sheetId="5" r:id="rId2"/>
+    <sheet name="prueba 3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
   <si>
     <t xml:space="preserve">Tipo de prueba </t>
   </si>
@@ -246,10 +248,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -262,9 +267,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -583,60 +585,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5467FEB1-E4CE-41DF-AF09-E96D6D5FEF05}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -656,165 +658,165 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -826,4 +828,378 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAA5066-6576-4027-B324-7EA61E5469D3}">
+  <dimension ref="B2:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8710560-FB1B-4E4F-821E-AF706076669B}">
+  <dimension ref="B2:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregan dos casos de prueba
</commit_message>
<xml_diff>
--- a/casos de prueba/casos de prueba.xlsx
+++ b/casos de prueba/casos de prueba.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbeja\Desktop\EntregaFinalCoder\Entrega_final_CodeHouse_Python\casos de prueba\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\clases python\Proyecto1\ENTREGA FINAL FINAL\Entrega_final_CodeHouse_Python\casos de prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC423438-1019-4083-805A-CB8D3DE609DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{216521C0-8688-43E0-9A96-A5931696C490}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Crud blog" sheetId="1" r:id="rId1"/>
-    <sheet name="prueba 2" sheetId="5" r:id="rId2"/>
-    <sheet name="prueba 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Crear usuario" sheetId="5" r:id="rId2"/>
+    <sheet name="Modificar usuario" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
   <si>
     <t xml:space="preserve">Tipo de prueba </t>
   </si>
@@ -148,12 +147,60 @@
   </si>
   <si>
     <t>se valida que se puede borrar un blog propio y que se pide una confirmacion para hacerlo</t>
+  </si>
+  <si>
+    <t>Melina Tarquini</t>
+  </si>
+  <si>
+    <t>Crear usuario</t>
+  </si>
+  <si>
+    <t>Modificar usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desde la url localhost:8000/blog ir a la opcion crear usuario </t>
+  </si>
+  <si>
+    <t>Tienen que aparecer todos los campos necesarios para crear el usuario</t>
+  </si>
+  <si>
+    <t>Iniciar sesión</t>
+  </si>
+  <si>
+    <t>Luego de crear el usuario aparece la opción de iniciar sesión con la url http://127.0.0.1:8000/blog/entrar/</t>
+  </si>
+  <si>
+    <t>Tiene que aparecer la página principal del blog junto con las opciones para listar blogs, crear un blog, ver perfil y salir</t>
+  </si>
+  <si>
+    <t>Ver perfil</t>
+  </si>
+  <si>
+    <t>desde la url http://127.0.0.1:8000/blog/ ir a la opción ver perfil</t>
+  </si>
+  <si>
+    <t>desde la url http://127.0.0.1:8000/user/perfil/ ir a la opción editar</t>
+  </si>
+  <si>
+    <t>Aparecerán los datos del usuario que pueden ser editados (nombre, apellido, usuario, dirección de email)</t>
+  </si>
+  <si>
+    <t>Se listarán los datos del usuario junto con las opciones: editar y cargar/editar Avatar</t>
+  </si>
+  <si>
+    <t>Perfil modificado</t>
+  </si>
+  <si>
+    <t>Aparecerá de nuevo el perfil del usuario pero con los datos actualizados en la url http://127.0.0.1:8000/user/perfil/</t>
+  </si>
+  <si>
+    <t>Una vez editado el usuario se debe hacer clic en Enviar (en la url http://127.0.0.1:8000/user/editar/)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -243,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -255,6 +302,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -582,65 +632,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5467FEB1-E4CE-41DF-AF09-E96D6D5FEF05}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="15" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
@@ -674,7 +724,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
@@ -691,7 +741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
@@ -708,7 +758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
@@ -725,7 +775,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
@@ -742,7 +792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
@@ -759,7 +809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -776,42 +826,42 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -831,59 +881,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAA5066-6576-4027-B324-7EA61E5469D3}">
-  <dimension ref="B2:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="15" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -900,110 +956,81 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1018,59 +1045,65 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8710560-FB1B-4E4F-821E-AF706076669B}">
-  <dimension ref="B2:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="15" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1087,110 +1120,98 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>